<commit_message>
Fix dashboard date filtering and Excel download functionality
- Fix dashboard controller: extend expense and income filtering from 30 to 60 days
- Fix Excel download: use buffer instead of file system for cloud compatibility
- Update frontend: use last60DaysExpense data structure
- Add debugging logs for better troubleshooting
- Update chart component title to 'Recent Expense Trends'
- Clean up unused SpendWise and test components
</commit_message>
<xml_diff>
--- a/backend/incomes_details.xlsx
+++ b/backend/incomes_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -438,29 +438,40 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Trading</v>
+        <v>Salary</v>
       </c>
       <c r="B4">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="C4" s="1">
-        <v>45860.22928240741</v>
+        <v>45862.22928240741</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>Trading</v>
+      </c>
+      <c r="B5">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45860.22928240741</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
         <v>Business</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>9000</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>45839.22928240741</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>